<commit_message>
updated sat scores and median household schema
</commit_message>
<xml_diff>
--- a/Excel Raw Data/median_household_income_by_county_2012-2017.xlsx
+++ b/Excel Raw Data/median_household_income_by_county_2012-2017.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anthonyrodriguez/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anthonyrodriguez/Desktop/GitHub/216finalproject/Excel Raw Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -332,22 +332,22 @@
     <t>County</t>
   </si>
   <si>
-    <t>Household Income 2012</t>
-  </si>
-  <si>
-    <t>Household Income 2013</t>
-  </si>
-  <si>
-    <t>Household Income 2014</t>
-  </si>
-  <si>
-    <t>Household Income 2015</t>
-  </si>
-  <si>
-    <t>Household Income 2016</t>
-  </si>
-  <si>
-    <t>Household Income 2017</t>
+    <t>Household_Income_2012</t>
+  </si>
+  <si>
+    <t>Household_Income_2014</t>
+  </si>
+  <si>
+    <t>Household_Income_2013</t>
+  </si>
+  <si>
+    <t>Household_Income_2015</t>
+  </si>
+  <si>
+    <t>Household_Income_2016</t>
+  </si>
+  <si>
+    <t>Household_Income_2017</t>
   </si>
 </sst>
 </file>
@@ -681,7 +681,7 @@
   <dimension ref="A1:G101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G101"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -692,7 +692,7 @@
     <col min="4" max="4" width="28" style="2" customWidth="1"/>
     <col min="5" max="5" width="28.1640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="26.83203125" customWidth="1"/>
-    <col min="7" max="7" width="23.83203125" customWidth="1"/>
+    <col min="7" max="7" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -703,10 +703,10 @@
         <v>101</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>103</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>104</v>

</xml_diff>